<commit_message>
change: Make 'save_with_drawings()' function.
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\Qiita記事\python\openpyxl-drawing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9F40D-1F00-423E-B8A8-0807A3F7EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6445AF15-6E2D-4324-B168-12CB80DDB64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -41,15 +42,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,19 +64,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,14 +113,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -109,7 +137,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="476250"/>
+          <a:off x="0" y="476250"/>
           <a:ext cx="2676525" cy="1590675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -188,17 +216,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533666</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>162147</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
+        <xdr:cNvPr id="2" name="図 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C11D322E-F9EC-50B8-3E26-AB4CD8F248E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85524137-50E1-BC47-8B63-449B90D4F656}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -207,16 +235,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
-              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -224,7 +243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="685800" y="238125"/>
-          <a:ext cx="7772400" cy="5829300"/>
+          <a:ext cx="1905266" cy="1590897"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -233,80 +252,71 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7772400" cy="285527"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="テキスト ボックス 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1B9DEF-4713-A232-CC59-90A8239D91AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="6067425"/>
-          <a:ext cx="7772400" cy="285527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="900">
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2" tooltip="https://www.flickr.com/photos/inucara/4341384538/"/>
-            </a:rPr>
-            <a:t>この写真</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="900"/>
-            <a:t> の作成者 不明な作成者 は </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="900">
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3" tooltip="https://creativecommons.org/licenses/by/3.0/"/>
-            </a:rPr>
-            <a:t>CC BY</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="900"/>
-            <a:t> のライセンスを許諾されています</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="図 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35052F01-A0D7-8B23-C515-BA225C754EAA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="Sheet3!$A$1:$C$2" spid="_x0000_s2051"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="685800" y="2143125"/>
+              <a:ext cx="1571625" cy="476250"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -575,11 +585,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1"/>
@@ -592,15 +603,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C78D397-F340-4767-BCCD-AD3D05B3B422}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="3" width="6.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>